<commit_message>
Added support for player teams - WIP
</commit_message>
<xml_diff>
--- a/dff.xlsx
+++ b/dff.xlsx
@@ -8325,10 +8325,10 @@
     <mergeCell ref="I2:I3"/>
     <mergeCell ref="B57:B60"/>
     <mergeCell ref="G18:G19"/>
+    <mergeCell ref="N23:N24"/>
     <mergeCell ref="E2:E3"/>
-    <mergeCell ref="N23:N24"/>
     <mergeCell ref="K2:K3"/>
-    <mergeCell ref="B32:B34"/>
+    <mergeCell ref="L23:L24"/>
     <mergeCell ref="K18:K19"/>
     <mergeCell ref="F13:F14"/>
     <mergeCell ref="B53:B56"/>
@@ -8350,11 +8350,11 @@
     <mergeCell ref="L8:L9"/>
     <mergeCell ref="D13:D14"/>
     <mergeCell ref="F23:F24"/>
-    <mergeCell ref="L23:L24"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="K8:K9"/>
     <mergeCell ref="K23:K24"/>
     <mergeCell ref="I13:I14"/>
+    <mergeCell ref="K13:K14"/>
     <mergeCell ref="M2:M3"/>
     <mergeCell ref="E23:E24"/>
     <mergeCell ref="N2:N3"/>
@@ -8363,7 +8363,6 @@
     <mergeCell ref="M13:M14"/>
     <mergeCell ref="N8:N9"/>
     <mergeCell ref="M8:M9"/>
-    <mergeCell ref="K13:K14"/>
     <mergeCell ref="D8:D9"/>
     <mergeCell ref="M18:M19"/>
     <mergeCell ref="I23:I24"/>
@@ -8371,30 +8370,31 @@
     <mergeCell ref="J2:J3"/>
     <mergeCell ref="H18:H19"/>
     <mergeCell ref="L2:L3"/>
-    <mergeCell ref="B49:B51"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="G8:G9"/>
     <mergeCell ref="N18:N19"/>
     <mergeCell ref="E13:E14"/>
     <mergeCell ref="B12:B15"/>
     <mergeCell ref="G13:G14"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="L13:L14"/>
+    <mergeCell ref="G23:G24"/>
+    <mergeCell ref="B49:B51"/>
     <mergeCell ref="B35:B37"/>
+    <mergeCell ref="B32:B34"/>
     <mergeCell ref="B46:B48"/>
-    <mergeCell ref="C18:C19"/>
     <mergeCell ref="B42:B44"/>
-    <mergeCell ref="C13:C14"/>
     <mergeCell ref="B39:B41"/>
-    <mergeCell ref="E18:E19"/>
     <mergeCell ref="D23:D24"/>
     <mergeCell ref="H23:H24"/>
     <mergeCell ref="J23:J24"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="G23:G24"/>
-    <mergeCell ref="L13:L14"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="B7:B10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="2">
@@ -21165,8 +21165,8 @@
     <mergeCell ref="H1:K1"/>
     <mergeCell ref="A63:A71"/>
     <mergeCell ref="A3:B3"/>
+    <mergeCell ref="B59:B61"/>
     <mergeCell ref="A6:A15"/>
-    <mergeCell ref="B59:B61"/>
     <mergeCell ref="B26:B33"/>
     <mergeCell ref="B38:B42"/>
     <mergeCell ref="B12:B15"/>
@@ -21191,10 +21191,10 @@
   <dimension ref="A1:P86"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="K74" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="5" topLeftCell="J72" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="P79" sqref="P79"/>
+      <selection pane="bottomRight" activeCell="C6" sqref="C6:P85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1"/>
@@ -22934,8 +22934,8 @@
     <mergeCell ref="H1:K1"/>
     <mergeCell ref="A63:A71"/>
     <mergeCell ref="A3:B3"/>
+    <mergeCell ref="B59:B61"/>
     <mergeCell ref="A6:A15"/>
-    <mergeCell ref="B59:B61"/>
     <mergeCell ref="B26:B33"/>
     <mergeCell ref="B38:B42"/>
     <mergeCell ref="B12:B15"/>
@@ -22979,8 +22979,8 @@
     <col min="12" max="12" width="1.6328125" style="160" customWidth="1"/>
     <col min="13" max="15" width="25.08984375" style="160" customWidth="1"/>
     <col min="16" max="16" width="26" style="160" customWidth="1"/>
-    <col min="17" max="29" width="12.6328125" style="160" customWidth="1"/>
-    <col min="30" max="16384" width="12.6328125" style="160"/>
+    <col min="17" max="40" width="12.6328125" style="160" customWidth="1"/>
+    <col min="41" max="16384" width="12.6328125" style="160"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15.5" customHeight="1">
@@ -24706,8 +24706,8 @@
     <mergeCell ref="H1:K1"/>
     <mergeCell ref="A63:A71"/>
     <mergeCell ref="A3:B3"/>
+    <mergeCell ref="B59:B61"/>
     <mergeCell ref="A6:A15"/>
-    <mergeCell ref="B59:B61"/>
     <mergeCell ref="B26:B33"/>
     <mergeCell ref="B38:B42"/>
     <mergeCell ref="B12:B15"/>

</xml_diff>